<commit_message>
Features - Upload completed
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Id</t>
   </si>
@@ -39,115 +39,16 @@
     <t>male</t>
   </si>
   <si>
-    <t>female</t>
-  </si>
-  <si>
     <t>ABC060</t>
   </si>
   <si>
-    <t>User3</t>
-  </si>
-  <si>
     <t>user3@gmail.com</t>
   </si>
   <si>
-    <t>ABC400</t>
-  </si>
-  <si>
-    <t>ABC401</t>
-  </si>
-  <si>
-    <t>ABC402</t>
-  </si>
-  <si>
-    <t>ABC403</t>
-  </si>
-  <si>
-    <t>ABC404</t>
-  </si>
-  <si>
-    <t>ABC405</t>
-  </si>
-  <si>
-    <t>ABC406</t>
-  </si>
-  <si>
-    <t>ABC407</t>
-  </si>
-  <si>
-    <t>User11</t>
-  </si>
-  <si>
-    <t>User12</t>
-  </si>
-  <si>
-    <t>User13</t>
-  </si>
-  <si>
-    <t>User14</t>
-  </si>
-  <si>
-    <t>User15</t>
-  </si>
-  <si>
-    <t>User16</t>
-  </si>
-  <si>
-    <t>User17</t>
-  </si>
-  <si>
-    <t>User18</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>Architect - Updated</t>
-  </si>
-  <si>
-    <t>user11@gmail.com</t>
-  </si>
-  <si>
-    <t>user12@gmail.com</t>
-  </si>
-  <si>
-    <t>user13@gmail.com</t>
-  </si>
-  <si>
-    <t>user14@gmail.com</t>
-  </si>
-  <si>
-    <t>user15@gmail.com</t>
-  </si>
-  <si>
-    <t>user16@gmail.com</t>
-  </si>
-  <si>
-    <t>user17@gmail.com</t>
-  </si>
-  <si>
-    <t>user18@gmail.com</t>
+    <t>Atif</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -465,9 +366,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -497,155 +400,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
         <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix - Create, Update and Id Generator
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
   <si>
     <t>Id</t>
   </si>
@@ -39,26 +39,313 @@
     <t>male</t>
   </si>
   <si>
-    <t>ABC060</t>
-  </si>
-  <si>
-    <t>user3@gmail.com</t>
-  </si>
-  <si>
-    <t>Atif</t>
-  </si>
-  <si>
-    <t>Test</t>
+    <t>First Name 11</t>
+  </si>
+  <si>
+    <t>First Name 12</t>
+  </si>
+  <si>
+    <t>First Name 13</t>
+  </si>
+  <si>
+    <t>First Name 14</t>
+  </si>
+  <si>
+    <t>First Name 15</t>
+  </si>
+  <si>
+    <t>First Name 16</t>
+  </si>
+  <si>
+    <t>First Name 17</t>
+  </si>
+  <si>
+    <t>First Name 18</t>
+  </si>
+  <si>
+    <t>First Name 19</t>
+  </si>
+  <si>
+    <t>First Name 20</t>
+  </si>
+  <si>
+    <t>First Name 21</t>
+  </si>
+  <si>
+    <t>First Name 22</t>
+  </si>
+  <si>
+    <t>First Name 23</t>
+  </si>
+  <si>
+    <t>First Name 24</t>
+  </si>
+  <si>
+    <t>Last Name 11</t>
+  </si>
+  <si>
+    <t>Last Name 12</t>
+  </si>
+  <si>
+    <t>Last Name 13</t>
+  </si>
+  <si>
+    <t>Last Name 14</t>
+  </si>
+  <si>
+    <t>Last Name 15</t>
+  </si>
+  <si>
+    <t>Last Name 16</t>
+  </si>
+  <si>
+    <t>Last Name 17</t>
+  </si>
+  <si>
+    <t>Last Name 18</t>
+  </si>
+  <si>
+    <t>Last Name 19</t>
+  </si>
+  <si>
+    <t>Last Name 20</t>
+  </si>
+  <si>
+    <t>Last Name 21</t>
+  </si>
+  <si>
+    <t>Last Name 22</t>
+  </si>
+  <si>
+    <t>Last Name 23</t>
+  </si>
+  <si>
+    <t>Last Name 24</t>
+  </si>
+  <si>
+    <t>First Name 25</t>
+  </si>
+  <si>
+    <t>Last Name 25</t>
+  </si>
+  <si>
+    <t>First Name 26</t>
+  </si>
+  <si>
+    <t>Last Name 26</t>
+  </si>
+  <si>
+    <t>First Name 27</t>
+  </si>
+  <si>
+    <t>Last Name 27</t>
+  </si>
+  <si>
+    <t>First Name 28</t>
+  </si>
+  <si>
+    <t>Last Name 28</t>
+  </si>
+  <si>
+    <t>First Name 29</t>
+  </si>
+  <si>
+    <t>Last Name 29</t>
+  </si>
+  <si>
+    <t>First Name 30</t>
+  </si>
+  <si>
+    <t>Last Name 30</t>
+  </si>
+  <si>
+    <t>First Name 31</t>
+  </si>
+  <si>
+    <t>Last Name 31</t>
+  </si>
+  <si>
+    <t>First Name 32</t>
+  </si>
+  <si>
+    <t>Last Name 32</t>
+  </si>
+  <si>
+    <t>First Name 33</t>
+  </si>
+  <si>
+    <t>Last Name 33</t>
+  </si>
+  <si>
+    <t>First Name 34</t>
+  </si>
+  <si>
+    <t>Last Name 34</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>user12@employer.com</t>
+  </si>
+  <si>
+    <t>user11@employer.com</t>
+  </si>
+  <si>
+    <t>user14@employer.com</t>
+  </si>
+  <si>
+    <t>user13@employer.com</t>
+  </si>
+  <si>
+    <t>user15@employer.com</t>
+  </si>
+  <si>
+    <t>user16@employer.com</t>
+  </si>
+  <si>
+    <t>user17@employer.com</t>
+  </si>
+  <si>
+    <t>user18@employer.com</t>
+  </si>
+  <si>
+    <t>user19@employer.com</t>
+  </si>
+  <si>
+    <t>user20@employer.com</t>
+  </si>
+  <si>
+    <t>user21@employer.com</t>
+  </si>
+  <si>
+    <t>user22@employer.com</t>
+  </si>
+  <si>
+    <t>user23@employer.com</t>
+  </si>
+  <si>
+    <t>user24@employer.com</t>
+  </si>
+  <si>
+    <t>user25@employer.com</t>
+  </si>
+  <si>
+    <t>user26@employer.com</t>
+  </si>
+  <si>
+    <t>user27@employer.com</t>
+  </si>
+  <si>
+    <t>user28@employer.com</t>
+  </si>
+  <si>
+    <t>user29@employer.com</t>
+  </si>
+  <si>
+    <t>user30@employer.com</t>
+  </si>
+  <si>
+    <t>user31@employer.com</t>
+  </si>
+  <si>
+    <t>user32@employer.com</t>
+  </si>
+  <si>
+    <t>user33@employer.com</t>
+  </si>
+  <si>
+    <t>user34@employer.com</t>
+  </si>
+  <si>
+    <t>EMP293718</t>
+  </si>
+  <si>
+    <t>EMP293719</t>
+  </si>
+  <si>
+    <t>EMP293720</t>
+  </si>
+  <si>
+    <t>EMP293721</t>
+  </si>
+  <si>
+    <t>EMP293722</t>
+  </si>
+  <si>
+    <t>EMP293723</t>
+  </si>
+  <si>
+    <t>EMP293724</t>
+  </si>
+  <si>
+    <t>EMP293725</t>
+  </si>
+  <si>
+    <t>EMP293726</t>
+  </si>
+  <si>
+    <t>EMP293727</t>
+  </si>
+  <si>
+    <t>EMP293728</t>
+  </si>
+  <si>
+    <t>EMP293729</t>
+  </si>
+  <si>
+    <t>EMP293730</t>
+  </si>
+  <si>
+    <t>EMP293731</t>
+  </si>
+  <si>
+    <t>EMP293732</t>
+  </si>
+  <si>
+    <t>EMP293733</t>
+  </si>
+  <si>
+    <t>EMP293734</t>
+  </si>
+  <si>
+    <t>EMP293735</t>
+  </si>
+  <si>
+    <t>EMP293736</t>
+  </si>
+  <si>
+    <t>EMP293737</t>
+  </si>
+  <si>
+    <t>EMP293738</t>
+  </si>
+  <si>
+    <t>EMP293739</t>
+  </si>
+  <si>
+    <t>EMP293740</t>
+  </si>
+  <si>
+    <t>EMP293741</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,13 +368,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -366,19 +656,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A10" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -400,23 +690,441 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E10" r:id="rId6"/>
+    <hyperlink ref="E7" r:id="rId7"/>
+    <hyperlink ref="E11" r:id="rId8"/>
+    <hyperlink ref="E8" r:id="rId9"/>
+    <hyperlink ref="E9" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId12"/>
+    <hyperlink ref="E14" r:id="rId13"/>
+    <hyperlink ref="E15" r:id="rId14"/>
+    <hyperlink ref="E16" r:id="rId15"/>
+    <hyperlink ref="E17" r:id="rId16"/>
+    <hyperlink ref="E18" r:id="rId17"/>
+    <hyperlink ref="E19" r:id="rId18"/>
+    <hyperlink ref="E20" r:id="rId19"/>
+    <hyperlink ref="E21" r:id="rId20"/>
+    <hyperlink ref="E22:E25" r:id="rId21" display="user30@employer.com"/>
+    <hyperlink ref="E22" r:id="rId22"/>
+    <hyperlink ref="E23" r:id="rId23"/>
+    <hyperlink ref="E24" r:id="rId24"/>
+    <hyperlink ref="E25" r:id="rId25"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>